<commit_message>
add q4 likert chart
</commit_message>
<xml_diff>
--- a/survey/responses.xlsx
+++ b/survey/responses.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stevao\Documents\workspace\vr_survey\survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B23355F-16D1-47D0-A195-7C51BD1F3420}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A84412-691F-46B1-A9A3-36933E013E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respostas ao formulário 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
+    <sheet name="heat map" sheetId="2" r:id="rId2"/>
+    <sheet name="Q4" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1768" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1782" uniqueCount="220">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -689,6 +690,9 @@
   </si>
   <si>
     <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t>Malfunction, or bugs contributes to a negative experience using VR (gaming, graphics) applications. Regarding the above statement you</t>
   </si>
 </sst>
 </file>
@@ -698,7 +702,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -725,6 +729,12 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -768,7 +778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -780,6 +790,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,6 +806,1683 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0"/>
+          <c:y val="0.19879051317680316"/>
+          <c:w val="0.96507936071483069"/>
+          <c:h val="0.7348444792817187"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q4'!$N$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Neutral</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Q4'!$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Malfunction, or bugs contributes to a negative experience using VR (gaming, graphics) applications. Regarding the above statement you</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q4'!$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-06FE-498F-920C-6AC4AD1002F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q4'!$L$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Disagree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>3</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-06FE-498F-920C-6AC4AD1002F9}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Q4'!$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Malfunction, or bugs contributes to a negative experience using VR (gaming, graphics) applications. Regarding the above statement you</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q4'!$L$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-06FE-498F-920C-6AC4AD1002F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q4'!$K$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Strongly Disagree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>2</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-06FE-498F-920C-6AC4AD1002F9}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="General" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Q4'!$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Malfunction, or bugs contributes to a negative experience using VR (gaming, graphics) applications. Regarding the above statement you</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q4'!$K$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-06FE-498F-920C-6AC4AD1002F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q4'!$M$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Disagree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q4'!$M$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-06FE-498F-920C-6AC4AD1002F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q4'!$O$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Neutral</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.8923710254155231E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>14</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-06FE-498F-920C-6AC4AD1002F9}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Q4'!$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Malfunction, or bugs contributes to a negative experience using VR (gaming, graphics) applications. Regarding the above statement you</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q4'!$O$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-06FE-498F-920C-6AC4AD1002F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q4'!$P$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Agree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2FF8CB32-361E-4E94-BB3E-3294D7CEEEF2}" type="VALUE">
+                      <a:rPr lang="en-US">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:pPr/>
+                      <a:t>[VALOR]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="pt-BR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-06FE-498F-920C-6AC4AD1002F9}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Q4'!$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Malfunction, or bugs contributes to a negative experience using VR (gaming, graphics) applications. Regarding the above statement you</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q4'!$P$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>39</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-06FE-498F-920C-6AC4AD1002F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q4'!$Q$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Strongly Agree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{874EB0D5-63E6-43B2-ADDC-A50E1208A880}" type="VALUE">
+                      <a:rPr lang="en-US">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:pPr/>
+                      <a:t>[VALOR]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="pt-BR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-06FE-498F-920C-6AC4AD1002F9}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Q4'!$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Malfunction, or bugs contributes to a negative experience using VR (gaming, graphics) applications. Regarding the above statement you</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q4'!$Q$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-06FE-498F-920C-6AC4AD1002F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="1143789552"/>
+        <c:axId val="1134281424"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1143789552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="1134281424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1134281424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1143789552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2247900</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B9CABEF-CA05-4ECF-B60E-F70FA1E4D5C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1000,9 +2688,9 @@
   </sheetPr>
   <dimension ref="A1:AD89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9047,4 +10735,109 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBD10A5-46D4-4D62-8FE0-F862DC9F4742}">
+  <dimension ref="A1:Q14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>39</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K13" t="s">
+        <v>72</v>
+      </c>
+      <c r="L13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" t="s">
+        <v>37</v>
+      </c>
+      <c r="N13" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J14" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="K14">
+        <v>-2</v>
+      </c>
+      <c r="L14">
+        <v>-3</v>
+      </c>
+      <c r="N14">
+        <v>-7</v>
+      </c>
+      <c r="O14">
+        <v>7</v>
+      </c>
+      <c r="P14">
+        <v>39</v>
+      </c>
+      <c r="Q14">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add analysis related to section 3
</commit_message>
<xml_diff>
--- a/survey/responses.xlsx
+++ b/survey/responses.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stevao\Documents\workspace\vr_survey\survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A84412-691F-46B1-A9A3-36933E013E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646EF5B3-66ED-477E-8346-FEF0B275F3BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respostas ao formulário 1" sheetId="1" r:id="rId1"/>
     <sheet name="heat map" sheetId="2" r:id="rId2"/>
     <sheet name="Q4" sheetId="3" r:id="rId3"/>
+    <sheet name="Section 3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1782" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="234">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -693,6 +694,48 @@
   </si>
   <si>
     <t>Malfunction, or bugs contributes to a negative experience using VR (gaming, graphics) applications. Regarding the above statement you</t>
+  </si>
+  <si>
+    <t>impeditive-technical</t>
+  </si>
+  <si>
+    <t>impeditive-nausea</t>
+  </si>
+  <si>
+    <t>impeditive-virtual_world</t>
+  </si>
+  <si>
+    <t>impeditive-real_world</t>
+  </si>
+  <si>
+    <t>impeditive-interaction</t>
+  </si>
+  <si>
+    <t>impeditive-peripherals</t>
+  </si>
+  <si>
+    <t>impeditive-inputs</t>
+  </si>
+  <si>
+    <t>Technical capabilities of the application</t>
+  </si>
+  <si>
+    <t>Nausea when using the app</t>
+  </si>
+  <si>
+    <t>Fidelity of virtual world</t>
+  </si>
+  <si>
+    <t>Awareness of real world</t>
+  </si>
+  <si>
+    <t>Interacting with real world objects</t>
+  </si>
+  <si>
+    <t>Interacting with real world peripherals</t>
+  </si>
+  <si>
+    <t>Providing input to the virtual world</t>
   </si>
 </sst>
 </file>
@@ -702,7 +745,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -736,8 +779,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -747,6 +797,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -778,7 +834,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -791,6 +847,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1899,6 +1959,1328 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.22580650950475112"/>
+          <c:y val="0.10288686793981869"/>
+          <c:w val="0.63437478127734037"/>
+          <c:h val="0.8627649750096873"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Section 3'!$E$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Neutral</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.2816396725038615E-2"/>
+                  <c:y val="-"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>23</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-FE98-40B9-8B1D-CFB07258C998}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.1390371929723598E-2"/>
+                  <c:y val="-"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>20</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-FE98-40B9-8B1D-CFB07258C998}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.4224595087557819E-2"/>
+                  <c:y val="-"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>29</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-FE98-40B9-8B1D-CFB07258C998}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.8502669473502664E-2"/>
+                  <c:y val="5.7246267103727409E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>32</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-FE98-40B9-8B1D-CFB07258C998}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.9946520701613182E-2"/>
+                  <c:y val="5.7246267103727409E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>26</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-FE98-40B9-8B1D-CFB07258C998}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.2798570292243111E-2"/>
+                  <c:y val="5.7246267103727409E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>27</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-FE98-40B9-8B1D-CFB07258C998}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.5264384997051384E-2"/>
+                  <c:y val="4.9174169005717972E-7"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>37</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-FE98-40B9-8B1D-CFB07258C998}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#;#" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Section 3'!$A$13:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Technical capabilities of the application</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nausea when using the app</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Fidelity of virtual world</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Awareness of real world</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Interacting with real world objects</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Interacting with real world peripherals</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Providing input to the virtual world</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Section 3'!$E$13:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>-11.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-14.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-13.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-18.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FE98-40B9-8B1D-CFB07258C998}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Section 3'!$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Disagree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#;#" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Section 3'!$A$13:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Technical capabilities of the application</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nausea when using the app</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Fidelity of virtual world</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Awareness of real world</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Interacting with real world objects</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Interacting with real world peripherals</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Providing input to the virtual world</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Section 3'!$C$13:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FE98-40B9-8B1D-CFB07258C998}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Section 3'!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Strongly Disagree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#;#" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Section 3'!$A$13:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Technical capabilities of the application</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nausea when using the app</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Fidelity of virtual world</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Awareness of real world</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Interacting with real world objects</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Interacting with real world peripherals</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Providing input to the virtual world</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Section 3'!$B$13:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FE98-40B9-8B1D-CFB07258C998}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Section 3'!$D$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Disagree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Section 3'!$D$13:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-FE98-40B9-8B1D-CFB07258C998}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Section 3'!$F$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Neutral</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Section 3'!$A$13:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Technical capabilities of the application</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nausea when using the app</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Fidelity of virtual world</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Awareness of real world</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Interacting with real world objects</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Interacting with real world peripherals</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Providing input to the virtual world</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Section 3'!$F$13:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FE98-40B9-8B1D-CFB07258C998}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Section 3'!$G$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Agree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Section 3'!$A$13:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Technical capabilities of the application</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nausea when using the app</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Fidelity of virtual world</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Awareness of real world</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Interacting with real world objects</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Interacting with real world peripherals</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Providing input to the virtual world</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Section 3'!$G$13:$G$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-FE98-40B9-8B1D-CFB07258C998}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Section 3'!$H$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Strongly Agree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Section 3'!$A$13:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Technical capabilities of the application</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nausea when using the app</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Fidelity of virtual world</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Awareness of real world</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Interacting with real world objects</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Interacting with real world peripherals</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Providing input to the virtual world</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Section 3'!$H$13:$H$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-FE98-40B9-8B1D-CFB07258C998}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="200150080"/>
+        <c:axId val="184726272"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="200150080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="184726272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="0"/>
+        <c:tickLblSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="184726272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="200150080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1939,7 +3321,552 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2485,6 +4412,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1323975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161923</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{666E2280-48EF-41A2-BAA6-6B20349AFBAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -2688,9 +4656,9 @@
   </sheetPr>
   <dimension ref="A1:AD89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N1" sqref="N1:T89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10741,7 +12709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBD10A5-46D4-4D62-8FE0-F862DC9F4742}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
@@ -10840,4 +12808,396 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18315CC9-46B0-4049-A8AA-9395E6FEC9AD}">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="47.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="10"/>
+      <c r="B1" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="10">
+        <v>4</v>
+      </c>
+      <c r="C2" s="10">
+        <v>10</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10">
+        <v>4</v>
+      </c>
+      <c r="F2" s="10">
+        <v>3</v>
+      </c>
+      <c r="G2" s="10">
+        <v>2</v>
+      </c>
+      <c r="H2" s="10">
+        <v>4</v>
+      </c>
+      <c r="I2" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10">
+        <v>16</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10">
+        <v>15</v>
+      </c>
+      <c r="F3" s="10">
+        <v>14</v>
+      </c>
+      <c r="G3" s="10">
+        <v>16</v>
+      </c>
+      <c r="H3" s="10">
+        <v>11</v>
+      </c>
+      <c r="I3" s="10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="10">
+        <v>23</v>
+      </c>
+      <c r="C4" s="10">
+        <v>20</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10">
+        <v>29</v>
+      </c>
+      <c r="F4" s="10">
+        <v>32</v>
+      </c>
+      <c r="G4" s="10">
+        <v>26</v>
+      </c>
+      <c r="H4" s="10">
+        <v>27</v>
+      </c>
+      <c r="I4" s="10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="10">
+        <v>47</v>
+      </c>
+      <c r="C5" s="10">
+        <v>18</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10">
+        <v>29</v>
+      </c>
+      <c r="F5" s="10">
+        <v>28</v>
+      </c>
+      <c r="G5" s="10">
+        <v>29</v>
+      </c>
+      <c r="H5" s="10">
+        <v>37</v>
+      </c>
+      <c r="I5" s="10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="10">
+        <v>12</v>
+      </c>
+      <c r="C6" s="10">
+        <v>24</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10">
+        <v>10</v>
+      </c>
+      <c r="F6" s="10">
+        <v>11</v>
+      </c>
+      <c r="G6" s="10">
+        <v>15</v>
+      </c>
+      <c r="H6" s="10">
+        <v>9</v>
+      </c>
+      <c r="I6" s="10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>227</v>
+      </c>
+      <c r="B13" s="10">
+        <v>-4</v>
+      </c>
+      <c r="C13" s="10">
+        <v>-2</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10">
+        <f>-23/2</f>
+        <v>-11.5</v>
+      </c>
+      <c r="F13" s="10">
+        <f>23/2</f>
+        <v>11.5</v>
+      </c>
+      <c r="G13" s="10">
+        <v>47</v>
+      </c>
+      <c r="H13" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>228</v>
+      </c>
+      <c r="B14" s="10">
+        <v>-10</v>
+      </c>
+      <c r="C14" s="10">
+        <v>-16</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10">
+        <f>-20/2</f>
+        <v>-10</v>
+      </c>
+      <c r="F14" s="10">
+        <f>20/2</f>
+        <v>10</v>
+      </c>
+      <c r="G14" s="10">
+        <v>18</v>
+      </c>
+      <c r="H14" s="10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>229</v>
+      </c>
+      <c r="B15" s="10">
+        <v>-4</v>
+      </c>
+      <c r="C15" s="10">
+        <v>-15</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10">
+        <f>-29/2</f>
+        <v>-14.5</v>
+      </c>
+      <c r="F15" s="10">
+        <f>29/2</f>
+        <v>14.5</v>
+      </c>
+      <c r="G15" s="10">
+        <v>29</v>
+      </c>
+      <c r="H15" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>230</v>
+      </c>
+      <c r="B16" s="10">
+        <v>-3</v>
+      </c>
+      <c r="C16" s="10">
+        <v>-14</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10">
+        <f>-32/2</f>
+        <v>-16</v>
+      </c>
+      <c r="F16" s="10">
+        <f>32/2</f>
+        <v>16</v>
+      </c>
+      <c r="G16" s="10">
+        <v>28</v>
+      </c>
+      <c r="H16" s="10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17" s="10">
+        <v>-2</v>
+      </c>
+      <c r="C17" s="10">
+        <v>-16</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10">
+        <f>-26/2</f>
+        <v>-13</v>
+      </c>
+      <c r="F17" s="10">
+        <f>26/2</f>
+        <v>13</v>
+      </c>
+      <c r="G17" s="10">
+        <v>29</v>
+      </c>
+      <c r="H17" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>232</v>
+      </c>
+      <c r="B18" s="10">
+        <v>-4</v>
+      </c>
+      <c r="C18" s="10">
+        <v>-11</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10">
+        <f>-27/2</f>
+        <v>-13.5</v>
+      </c>
+      <c r="F18" s="10">
+        <f>27/2</f>
+        <v>13.5</v>
+      </c>
+      <c r="G18" s="10">
+        <v>37</v>
+      </c>
+      <c r="H18" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>233</v>
+      </c>
+      <c r="B19" s="10">
+        <v>-1</v>
+      </c>
+      <c r="C19" s="10">
+        <v>-13</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10">
+        <f>-37/2</f>
+        <v>-18.5</v>
+      </c>
+      <c r="F19" s="10">
+        <f>37/2</f>
+        <v>18.5</v>
+      </c>
+      <c r="G19" s="10">
+        <v>24</v>
+      </c>
+      <c r="H19" s="10">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add a table related to section 4 results
</commit_message>
<xml_diff>
--- a/survey/responses.xlsx
+++ b/survey/responses.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stevao\Documents\workspace\vr_survey\survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646EF5B3-66ED-477E-8346-FEF0B275F3BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21805C05-489C-49C3-9FC0-2BD5B8BA6C9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respostas ao formulário 1" sheetId="1" r:id="rId1"/>
     <sheet name="heat map" sheetId="2" r:id="rId2"/>
     <sheet name="Q4" sheetId="3" r:id="rId3"/>
     <sheet name="Section 3" sheetId="4" r:id="rId4"/>
+    <sheet name="Section 4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="292">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -717,25 +718,199 @@
     <t>impeditive-inputs</t>
   </si>
   <si>
-    <t>Technical capabilities of the application</t>
-  </si>
-  <si>
-    <t>Nausea when using the app</t>
-  </si>
-  <si>
-    <t>Fidelity of virtual world</t>
-  </si>
-  <si>
-    <t>Awareness of real world</t>
-  </si>
-  <si>
-    <t>Interacting with real world objects</t>
-  </si>
-  <si>
-    <t>Interacting with real world peripherals</t>
-  </si>
-  <si>
-    <t>Providing input to the virtual world</t>
+    <t>A1:</t>
+  </si>
+  <si>
+    <t>A2:</t>
+  </si>
+  <si>
+    <t>A3:</t>
+  </si>
+  <si>
+    <t>A4:</t>
+  </si>
+  <si>
+    <t>A5:</t>
+  </si>
+  <si>
+    <t>A6:</t>
+  </si>
+  <si>
+    <t>A7:</t>
+  </si>
+  <si>
+    <t>Missing geometry</t>
+  </si>
+  <si>
+    <t>Stuck (unable to move)</t>
+  </si>
+  <si>
+    <t>Objects floating abnormally</t>
+  </si>
+  <si>
+    <t>Impossible to pile objects</t>
+  </si>
+  <si>
+    <t>Fault characteristic</t>
+  </si>
+  <si>
+    <t>Occurrence among responders</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>66/88</t>
+  </si>
+  <si>
+    <t>31/88</t>
+  </si>
+  <si>
+    <t>14/88</t>
+  </si>
+  <si>
+    <t>42/88</t>
+  </si>
+  <si>
+    <t>59/88</t>
+  </si>
+  <si>
+    <t>35/88</t>
+  </si>
+  <si>
+    <t>20/88</t>
+  </si>
+  <si>
+    <t>58/88</t>
+  </si>
+  <si>
+    <t>56/88</t>
+  </si>
+  <si>
+    <t>40/88</t>
+  </si>
+  <si>
+    <t>37/88</t>
+  </si>
+  <si>
+    <t>36/88</t>
+  </si>
+  <si>
+    <t>39/88</t>
+  </si>
+  <si>
+    <t>64/88</t>
+  </si>
+  <si>
+    <t>26/88</t>
+  </si>
+  <si>
+    <t>16/88</t>
+  </si>
+  <si>
+    <t>47/88</t>
+  </si>
+  <si>
+    <t>43/88</t>
+  </si>
+  <si>
+    <t>45/88</t>
+  </si>
+  <si>
+    <t>38/88</t>
+  </si>
+  <si>
+    <t>30/88</t>
+  </si>
+  <si>
+    <t>34/88</t>
+  </si>
+  <si>
+    <t>18/88</t>
+  </si>
+  <si>
+    <t>51/88</t>
+  </si>
+  <si>
+    <t>28/88</t>
+  </si>
+  <si>
+    <t>39.1%</t>
+  </si>
+  <si>
+    <t>20.7%</t>
+  </si>
+  <si>
+    <t>43.7%</t>
+  </si>
+  <si>
+    <t>58.6%</t>
+  </si>
+  <si>
+    <t>32.2%</t>
+  </si>
+  <si>
+    <t>35.2%</t>
+  </si>
+  <si>
+    <t>40.9%</t>
+  </si>
+  <si>
+    <t>51.1%</t>
+  </si>
+  <si>
+    <t>43.3%</t>
+  </si>
+  <si>
+    <t>34.1%</t>
+  </si>
+  <si>
+    <t>29.5%</t>
+  </si>
+  <si>
+    <t>18.2%</t>
+  </si>
+  <si>
+    <t>53.4%</t>
+  </si>
+  <si>
+    <t>48.9%</t>
+  </si>
+  <si>
+    <t>45.9%</t>
+  </si>
+  <si>
+    <t>75.3%</t>
+  </si>
+  <si>
+    <t>39.8%</t>
+  </si>
+  <si>
+    <t>65.9%</t>
+  </si>
+  <si>
+    <t>15.9%</t>
+  </si>
+  <si>
+    <t>63.6%</t>
+  </si>
+  <si>
+    <t>45.5%</t>
+  </si>
+  <si>
+    <t>67.8%</t>
+  </si>
+  <si>
+    <t>40.2%</t>
+  </si>
+  <si>
+    <t>76.7%</t>
+  </si>
+  <si>
+    <t>16.3%</t>
+  </si>
+  <si>
+    <t>48.8%</t>
   </si>
 </sst>
 </file>
@@ -834,7 +1009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -851,6 +1026,19 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2022,7 +2210,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="2.2816396725038615E-2"/>
-                  <c:y val="-"/>
+                  <c:y val="0"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -2057,7 +2245,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="2.1390371929723598E-2"/>
-                  <c:y val="-"/>
+                  <c:y val="0"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -2092,7 +2280,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="3.4224595087557819E-2"/>
-                  <c:y val="-"/>
+                  <c:y val="0"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -2325,25 +2513,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Technical capabilities of the application</c:v>
+                  <c:v>A1:</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Nausea when using the app</c:v>
+                  <c:v>A2:</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Fidelity of virtual world</c:v>
+                  <c:v>A3:</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Awareness of real world</c:v>
+                  <c:v>A4:</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Interacting with real world objects</c:v>
+                  <c:v>A5:</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Interacting with real world peripherals</c:v>
+                  <c:v>A6:</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Providing input to the virtual world</c:v>
+                  <c:v>A7:</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2475,25 +2663,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Technical capabilities of the application</c:v>
+                  <c:v>A1:</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Nausea when using the app</c:v>
+                  <c:v>A2:</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Fidelity of virtual world</c:v>
+                  <c:v>A3:</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Awareness of real world</c:v>
+                  <c:v>A4:</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Interacting with real world objects</c:v>
+                  <c:v>A5:</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Interacting with real world peripherals</c:v>
+                  <c:v>A6:</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Providing input to the virtual world</c:v>
+                  <c:v>A7:</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2624,25 +2812,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Technical capabilities of the application</c:v>
+                  <c:v>A1:</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Nausea when using the app</c:v>
+                  <c:v>A2:</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Fidelity of virtual world</c:v>
+                  <c:v>A3:</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Awareness of real world</c:v>
+                  <c:v>A4:</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Interacting with real world objects</c:v>
+                  <c:v>A5:</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Interacting with real world peripherals</c:v>
+                  <c:v>A6:</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Providing input to the virtual world</c:v>
+                  <c:v>A7:</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2757,25 +2945,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Technical capabilities of the application</c:v>
+                  <c:v>A1:</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Nausea when using the app</c:v>
+                  <c:v>A2:</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Fidelity of virtual world</c:v>
+                  <c:v>A3:</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Awareness of real world</c:v>
+                  <c:v>A4:</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Interacting with real world objects</c:v>
+                  <c:v>A5:</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Interacting with real world peripherals</c:v>
+                  <c:v>A6:</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Providing input to the virtual world</c:v>
+                  <c:v>A7:</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2906,25 +3094,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Technical capabilities of the application</c:v>
+                  <c:v>A1:</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Nausea when using the app</c:v>
+                  <c:v>A2:</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Fidelity of virtual world</c:v>
+                  <c:v>A3:</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Awareness of real world</c:v>
+                  <c:v>A4:</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Interacting with real world objects</c:v>
+                  <c:v>A5:</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Interacting with real world peripherals</c:v>
+                  <c:v>A6:</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Providing input to the virtual world</c:v>
+                  <c:v>A7:</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3051,25 +3239,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Technical capabilities of the application</c:v>
+                  <c:v>A1:</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Nausea when using the app</c:v>
+                  <c:v>A2:</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Fidelity of virtual world</c:v>
+                  <c:v>A3:</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Awareness of real world</c:v>
+                  <c:v>A4:</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Interacting with real world objects</c:v>
+                  <c:v>A5:</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Interacting with real world peripherals</c:v>
+                  <c:v>A6:</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Providing input to the virtual world</c:v>
+                  <c:v>A7:</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3126,7 +3314,7 @@
       <c:catAx>
         <c:axId val="200150080"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3152,7 +3340,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1300" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3181,7 +3369,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3221,7 +3409,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4417,15 +4605,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1323975</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>161923</xdr:rowOff>
+      <xdr:colOff>2209800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114298</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4656,9 +4844,9 @@
   </sheetPr>
   <dimension ref="A1:AD89"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1" sqref="N1:T89"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U1" sqref="U1:AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12814,8 +13002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18315CC9-46B0-4049-A8AA-9395E6FEC9AD}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13014,7 +13202,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="14" t="s">
         <v>227</v>
       </c>
       <c r="B13" s="10">
@@ -13040,7 +13228,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>228</v>
       </c>
       <c r="B14" s="10">
@@ -13066,7 +13254,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>229</v>
       </c>
       <c r="B15" s="10">
@@ -13092,7 +13280,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>230</v>
       </c>
       <c r="B16" s="10">
@@ -13118,7 +13306,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>231</v>
       </c>
       <c r="B17" s="10">
@@ -13144,7 +13332,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>232</v>
       </c>
       <c r="B18" s="10">
@@ -13170,7 +13358,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>233</v>
       </c>
       <c r="B19" s="10">
@@ -13200,4 +13388,465 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A33B3DC-5D62-4CE9-B4E8-15020225A4F9}">
+  <dimension ref="A1:C42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection sqref="A1:C42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="C17" s="18">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="C33" s="18">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="C37" s="18">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="C40" s="18">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>291</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A29:C29"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>